<commit_message>
Added SHOPPERS Table to the Database
Also updated the Excel Spreadsheet that I'm using to keep track of the Gantt Chart for the week.
</commit_message>
<xml_diff>
--- a/Week 7 Gantt Chart.xlsx
+++ b/Week 7 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16CB51AF-1EF2-40D8-86E9-EF551429E588}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A48F0AA7-66A0-447C-B39D-48145EF30568}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -744,7 +744,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -976,56 +976,50 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1327,6 +1321,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1595,7 +1593,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1643,110 +1641,110 @@
       <c r="A3" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="88">
+      <c r="D3" s="97"/>
+      <c r="E3" s="95">
         <v>44951</v>
       </c>
-      <c r="F3" s="88"/>
+      <c r="F3" s="95"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="83" t="s">
+      <c r="B4" s="91"/>
+      <c r="C4" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="97"/>
       <c r="E4" s="7">
         <v>5</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="92">
         <f>I5</f>
         <v>44977</v>
       </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="85">
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
+      <c r="M4" s="93"/>
+      <c r="N4" s="93"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="92">
         <f>P5</f>
         <v>44984</v>
       </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="85">
+      <c r="Q4" s="93"/>
+      <c r="R4" s="93"/>
+      <c r="S4" s="93"/>
+      <c r="T4" s="93"/>
+      <c r="U4" s="93"/>
+      <c r="V4" s="94"/>
+      <c r="W4" s="92">
         <f>W5</f>
         <v>44991</v>
       </c>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="85">
+      <c r="X4" s="93"/>
+      <c r="Y4" s="93"/>
+      <c r="Z4" s="93"/>
+      <c r="AA4" s="93"/>
+      <c r="AB4" s="93"/>
+      <c r="AC4" s="94"/>
+      <c r="AD4" s="92">
         <f>AD5</f>
         <v>44998</v>
       </c>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="85">
+      <c r="AE4" s="93"/>
+      <c r="AF4" s="93"/>
+      <c r="AG4" s="93"/>
+      <c r="AH4" s="93"/>
+      <c r="AI4" s="93"/>
+      <c r="AJ4" s="94"/>
+      <c r="AK4" s="92">
         <f>AK5</f>
         <v>45005</v>
       </c>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="85">
+      <c r="AL4" s="93"/>
+      <c r="AM4" s="93"/>
+      <c r="AN4" s="93"/>
+      <c r="AO4" s="93"/>
+      <c r="AP4" s="93"/>
+      <c r="AQ4" s="94"/>
+      <c r="AR4" s="92">
         <f>AR5</f>
         <v>45012</v>
       </c>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="86"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="85">
+      <c r="AS4" s="93"/>
+      <c r="AT4" s="93"/>
+      <c r="AU4" s="93"/>
+      <c r="AV4" s="93"/>
+      <c r="AW4" s="93"/>
+      <c r="AX4" s="94"/>
+      <c r="AY4" s="92">
         <f>AY5</f>
         <v>45019</v>
       </c>
-      <c r="AZ4" s="86"/>
-      <c r="BA4" s="86"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="86"/>
-      <c r="BD4" s="86"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="85">
+      <c r="AZ4" s="93"/>
+      <c r="BA4" s="93"/>
+      <c r="BB4" s="93"/>
+      <c r="BC4" s="93"/>
+      <c r="BD4" s="93"/>
+      <c r="BE4" s="94"/>
+      <c r="BF4" s="92">
         <f>BF5</f>
         <v>45026</v>
       </c>
-      <c r="BG4" s="86"/>
-      <c r="BH4" s="86"/>
-      <c r="BI4" s="86"/>
-      <c r="BJ4" s="86"/>
-      <c r="BK4" s="86"/>
-      <c r="BL4" s="87"/>
+      <c r="BG4" s="93"/>
+      <c r="BH4" s="93"/>
+      <c r="BI4" s="93"/>
+      <c r="BJ4" s="93"/>
+      <c r="BK4" s="93"/>
+      <c r="BL4" s="94"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
@@ -2375,7 +2373,7 @@
       <c r="A9" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="90" t="s">
+      <c r="B9" s="83" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="70" t="s">
@@ -2457,14 +2455,14 @@
       <c r="A10" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="83" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="70" t="s">
         <v>47</v>
       </c>
       <c r="D10" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="64">
         <f>F9</f>
@@ -2538,7 +2536,7 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="83" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="70" t="s">
@@ -2692,14 +2690,14 @@
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="59"/>
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="84" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="72" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="27">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="E13" s="65">
         <f>E9</f>
@@ -2773,7 +2771,7 @@
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="58"/>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="90" t="s">
         <v>71</v>
       </c>
       <c r="C14" s="72" t="s">
@@ -2854,7 +2852,7 @@
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="58"/>
-      <c r="B15" s="91" t="s">
+      <c r="B15" s="84" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="72" t="s">
@@ -2935,7 +2933,7 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="58"/>
-      <c r="B16" s="91" t="s">
+      <c r="B16" s="84" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="72" t="s">
@@ -3016,7 +3014,7 @@
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="58"/>
-      <c r="B17" s="91" t="s">
+      <c r="B17" s="84" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="72" t="s">
@@ -3094,7 +3092,7 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="58"/>
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="84" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="72" t="s">
@@ -3172,7 +3170,7 @@
     </row>
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="58"/>
-      <c r="B19" s="91" t="s">
+      <c r="B19" s="84" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="72" t="s">
@@ -3250,7 +3248,7 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="58"/>
-      <c r="B20" s="91" t="s">
+      <c r="B20" s="84" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="72" t="s">
@@ -3401,7 +3399,7 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="58"/>
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="85" t="s">
         <v>72</v>
       </c>
       <c r="C22" s="74" t="s">
@@ -3482,7 +3480,7 @@
     </row>
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="58"/>
-      <c r="B23" s="92" t="s">
+      <c r="B23" s="85" t="s">
         <v>56</v>
       </c>
       <c r="C23" s="74" t="s">
@@ -3636,7 +3634,7 @@
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="58"/>
-      <c r="B25" s="93" t="s">
+      <c r="B25" s="86" t="s">
         <v>59</v>
       </c>
       <c r="C25" s="76" t="s">
@@ -3717,7 +3715,7 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="58"/>
-      <c r="B26" s="93" t="s">
+      <c r="B26" s="86" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="76" t="s">
@@ -3798,10 +3796,10 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="58"/>
-      <c r="B27" s="95" t="s">
+      <c r="B27" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="96" t="s">
+      <c r="C27" s="89" t="s">
         <v>58</v>
       </c>
       <c r="D27" s="37">
@@ -3879,7 +3877,7 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="58"/>
-      <c r="B28" s="95" t="s">
+      <c r="B28" s="88" t="s">
         <v>61</v>
       </c>
       <c r="C28" s="76" t="s">
@@ -3960,10 +3958,10 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="58"/>
-      <c r="B29" s="94" t="s">
+      <c r="B29" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="96" t="s">
+      <c r="C29" s="89" t="s">
         <v>63</v>
       </c>
       <c r="D29" s="37">
@@ -4038,10 +4036,10 @@
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="58"/>
-      <c r="B30" s="97" t="s">
+      <c r="B30" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="96" t="s">
+      <c r="C30" s="89" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="37">
@@ -4116,14 +4114,14 @@
     </row>
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="58"/>
-      <c r="B31" s="97" t="s">
+      <c r="B31" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="96" t="s">
+      <c r="C31" s="89" t="s">
         <v>46</v>
       </c>
       <c r="D31" s="37">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E31" s="67">
         <f>E13</f>
@@ -4194,10 +4192,10 @@
     </row>
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="58"/>
-      <c r="B32" s="97" t="s">
+      <c r="B32" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="96" t="s">
+      <c r="C32" s="89" t="s">
         <v>47</v>
       </c>
       <c r="D32" s="37">
@@ -4272,10 +4270,10 @@
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="58"/>
-      <c r="B33" s="97" t="s">
+      <c r="B33" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="96" t="s">
+      <c r="C33" s="89" t="s">
         <v>47</v>
       </c>
       <c r="D33" s="37">
@@ -4350,10 +4348,10 @@
     </row>
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="58"/>
-      <c r="B34" s="97" t="s">
+      <c r="B34" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="96" t="s">
+      <c r="C34" s="89" t="s">
         <v>47</v>
       </c>
       <c r="D34" s="37">
@@ -4428,10 +4426,10 @@
     </row>
     <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="58"/>
-      <c r="B35" s="97" t="s">
+      <c r="B35" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="96" t="s">
+      <c r="C35" s="89" t="s">
         <v>47</v>
       </c>
       <c r="D35" s="37">
@@ -4506,10 +4504,10 @@
     </row>
     <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="58"/>
-      <c r="B36" s="97" t="s">
+      <c r="B36" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="96" t="s">
+      <c r="C36" s="89" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="37">
@@ -4584,10 +4582,10 @@
     </row>
     <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="58"/>
-      <c r="B37" s="94" t="s">
+      <c r="B37" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="96" t="s">
+      <c r="C37" s="89" t="s">
         <v>47</v>
       </c>
       <c r="D37" s="37">

</xml_diff>

<commit_message>
Fixing Build Error from previous Commit and Encryption
Last commit I forgot to build my code so I didn't know that it wouldn't even compile, but I got it to work now.

Also on the side I fixed the md5 encryption so we should be able to have that working WITHOUT needing to use the boost library.
</commit_message>
<xml_diff>
--- a/Week 7 Gantt Chart.xlsx
+++ b/Week 7 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A48F0AA7-66A0-447C-B39D-48145EF30568}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BBBD714-285E-4BEF-823E-A8D4281BF8DC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -208,18 +208,12 @@
     <t>Edit Database</t>
   </si>
   <si>
-    <t>Create "SHOPPERS" Table</t>
-  </si>
-  <si>
     <t>Create this Gantt Chart</t>
   </si>
   <si>
     <t>Editing Shopping Menu</t>
   </si>
   <si>
-    <t>Create the Menu if its not yet made</t>
-  </si>
-  <si>
     <t>Chris</t>
   </si>
   <si>
@@ -229,9 +223,6 @@
     <t>Mike</t>
   </si>
   <si>
-    <t>Add new shopper to database</t>
-  </si>
-  <si>
     <t>Add "Purchase" Option to Menu</t>
   </si>
   <si>
@@ -280,9 +271,6 @@
     <t>Issue ID 8: Import files into database</t>
   </si>
   <si>
-    <t>Modify Quanty on Hand to Random #</t>
-  </si>
-  <si>
     <t>Remove Uneeded Comments</t>
   </si>
   <si>
@@ -308,6 +296,27 @@
   </si>
   <si>
     <t>Get Admin Login Errors be More Exact</t>
+  </si>
+  <si>
+    <t>Add new shopper to DB</t>
+  </si>
+  <si>
+    <t>Modify Qantity to a Random #</t>
+  </si>
+  <si>
+    <t>Create SHOPPERS Table</t>
+  </si>
+  <si>
+    <t>Create the Menu if not made yet</t>
+  </si>
+  <si>
+    <t>Legend:</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Not Completed</t>
   </si>
 </sst>
 </file>
@@ -513,7 +522,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -590,6 +599,18 @@
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -744,7 +765,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1020,6 +1041,21 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1591,9 +1627,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BL42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1652,6 +1688,32 @@
         <v>44951</v>
       </c>
       <c r="F3" s="95"/>
+      <c r="I3" s="99" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="101" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3" s="101"/>
+      <c r="O3" s="101"/>
+      <c r="P3" s="101"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="100"/>
+      <c r="S3" s="102" t="s">
+        <v>78</v>
+      </c>
+      <c r="T3" s="102"/>
+      <c r="U3" s="102"/>
+      <c r="V3" s="102"/>
+      <c r="W3" s="102"/>
+      <c r="X3" s="102"/>
+      <c r="Y3" s="100"/>
+      <c r="Z3" s="100"/>
+      <c r="AA3" s="100"/>
+      <c r="AB3" s="100"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
@@ -2374,10 +2436,10 @@
         <v>37</v>
       </c>
       <c r="B9" s="83" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9" s="22">
         <v>0.85</v>
@@ -2456,10 +2518,10 @@
         <v>33</v>
       </c>
       <c r="B10" s="83" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="22">
         <v>1</v>
@@ -2537,10 +2599,10 @@
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
       <c r="B11" s="83" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11" s="22">
         <v>1</v>
@@ -2620,7 +2682,7 @@
         <v>34</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="71"/>
       <c r="D12" s="24"/>
@@ -2691,10 +2753,10 @@
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="59"/>
       <c r="B13" s="84" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C13" s="72" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" s="27">
         <v>0.8</v>
@@ -2772,21 +2834,21 @@
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="58"/>
       <c r="B14" s="90" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C14" s="72" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" s="27">
         <v>0</v>
       </c>
       <c r="E14" s="65">
-        <f>F13</f>
-        <v>44981</v>
+        <f>E9+2</f>
+        <v>44982</v>
       </c>
       <c r="F14" s="65">
         <f>E14</f>
-        <v>44981</v>
+        <v>44982</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17">
@@ -2853,16 +2915,16 @@
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="58"/>
       <c r="B15" s="84" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="C15" s="72" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="27">
         <v>0</v>
       </c>
       <c r="E15" s="65">
-        <f>F14</f>
+        <f>F13</f>
         <v>44981</v>
       </c>
       <c r="F15" s="65">
@@ -2934,21 +2996,21 @@
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="58"/>
       <c r="B16" s="84" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C16" s="72" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D16" s="27">
         <v>0</v>
       </c>
       <c r="E16" s="65">
         <f>F14</f>
-        <v>44981</v>
+        <v>44982</v>
       </c>
       <c r="F16" s="65">
         <f>E16+1</f>
-        <v>44982</v>
+        <v>44983</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17">
@@ -3015,21 +3077,21 @@
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="58"/>
       <c r="B17" s="84" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C17" s="72" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D17" s="27">
         <v>0</v>
       </c>
       <c r="E17" s="65">
         <f>F16</f>
-        <v>44982</v>
+        <v>44983</v>
       </c>
       <c r="F17" s="65">
         <f>E17</f>
-        <v>44982</v>
+        <v>44983</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
@@ -3092,11 +3154,11 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="58"/>
-      <c r="B18" s="84" t="s">
-        <v>53</v>
+      <c r="B18" s="98" t="s">
+        <v>50</v>
       </c>
       <c r="C18" s="72" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18" s="27">
         <v>0</v>
@@ -3171,10 +3233,10 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="58"/>
       <c r="B19" s="84" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C19" s="72" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D19" s="27">
         <v>0</v>
@@ -3249,21 +3311,21 @@
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="58"/>
       <c r="B20" s="84" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" s="72" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D20" s="27">
         <v>0</v>
       </c>
       <c r="E20" s="65">
         <f>F17</f>
-        <v>44982</v>
+        <v>44983</v>
       </c>
       <c r="F20" s="65">
         <f>E20</f>
-        <v>44982</v>
+        <v>44983</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
@@ -3329,7 +3391,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C21" s="73"/>
       <c r="D21" s="29"/>
@@ -3400,21 +3462,21 @@
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="58"/>
       <c r="B22" s="85" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C22" s="74" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" s="32">
         <v>0</v>
       </c>
       <c r="E22" s="66">
         <f>F20+1</f>
-        <v>44983</v>
+        <v>44984</v>
       </c>
       <c r="F22" s="66">
         <f>E22+1</f>
-        <v>44984</v>
+        <v>44985</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
@@ -3481,16 +3543,16 @@
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="58"/>
       <c r="B23" s="85" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C23" s="74" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D23" s="32">
         <v>0</v>
       </c>
       <c r="E23" s="66">
-        <f>E22</f>
+        <f>F19+1</f>
         <v>44983</v>
       </c>
       <c r="F23" s="66">
@@ -3564,7 +3626,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C24" s="75"/>
       <c r="D24" s="34"/>
@@ -3635,10 +3697,10 @@
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="58"/>
       <c r="B25" s="86" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C25" s="76" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25" s="37">
         <v>0</v>
@@ -3716,10 +3778,10 @@
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="58"/>
       <c r="B26" s="86" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C26" s="76" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D26" s="37">
         <v>0</v>
@@ -3797,10 +3859,10 @@
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="58"/>
       <c r="B27" s="88" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C27" s="89" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D27" s="37">
         <v>0.05</v>
@@ -3878,10 +3940,10 @@
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="58"/>
       <c r="B28" s="88" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C28" s="76" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D28" s="37">
         <v>0</v>
@@ -3959,10 +4021,10 @@
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="58"/>
       <c r="B29" s="87" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C29" s="89" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D29" s="37">
         <v>0</v>
@@ -4037,13 +4099,13 @@
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="58"/>
       <c r="B30" s="86" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C30" s="89" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D30" s="37">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E30" s="67">
         <f>F32</f>
@@ -4115,10 +4177,10 @@
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="58"/>
       <c r="B31" s="86" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C31" s="89" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D31" s="37">
         <v>0.8</v>
@@ -4193,10 +4255,10 @@
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="58"/>
       <c r="B32" s="86" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32" s="89" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D32" s="37">
         <v>0.5</v>
@@ -4271,10 +4333,10 @@
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="58"/>
       <c r="B33" s="86" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C33" s="89" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D33" s="37">
         <v>0</v>
@@ -4349,10 +4411,10 @@
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="58"/>
       <c r="B34" s="86" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C34" s="89" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D34" s="37">
         <v>0</v>
@@ -4427,13 +4489,13 @@
     <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="58"/>
       <c r="B35" s="86" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C35" s="89" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D35" s="37">
-        <v>0.01</v>
+        <v>0.2</v>
       </c>
       <c r="E35" s="67">
         <f>E9</f>
@@ -4505,10 +4567,10 @@
     <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="58"/>
       <c r="B36" s="86" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C36" s="89" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D36" s="37">
         <v>0.1</v>
@@ -4583,10 +4645,10 @@
     <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="58"/>
       <c r="B37" s="87" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C37" s="89" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D37" s="37">
         <v>0.01</v>
@@ -4813,7 +4875,7 @@
       <c r="C42" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4826,6 +4888,8 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="S3:X3"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D39">
     <cfRule type="dataBar" priority="14">

</xml_diff>

<commit_message>
Finishing Testing on Previous Two Weeks of Code
Several changes and fixes were made all across the codebase to make sure that everything is working properly. These changes include:

Front-End:
 + Uncommenting out the use of the hashing function for the password
 ~ Adjusting the input validation for importing books so that the user can actually select yes or no
 ~ Changing the use of isStringInt() to isStringFloat() for variables that are meant to be floating point numbers
 ~ Allowing users to enter in a MSRP above 0 instead of between two values.

Utilities:
 ~ Changing the name of isNumber() to isStringInt() in order to be more descriptive
 + Adding in the isStringFloat() function to allow us to test floating point numbers as well as integer numbers.
</commit_message>
<xml_diff>
--- a/Week 7 Gantt Chart.xlsx
+++ b/Week 7 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="102" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BBBD714-285E-4BEF-823E-A8D4281BF8DC}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{069BA28C-D5F5-4D3D-8FB0-4597D0772E53}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -765,7 +765,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1041,15 +1041,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1628,8 +1619,8 @@
   <dimension ref="A1:BL42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1688,32 +1679,32 @@
         <v>44951</v>
       </c>
       <c r="F3" s="95"/>
-      <c r="I3" s="99" t="s">
+      <c r="I3" s="3" t="s">
         <v>76</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="101" t="s">
+      <c r="M3" s="98" t="s">
         <v>77</v>
       </c>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="101"/>
-      <c r="Q3" s="101"/>
-      <c r="R3" s="100"/>
-      <c r="S3" s="102" t="s">
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="98"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="T3" s="102"/>
-      <c r="U3" s="102"/>
-      <c r="V3" s="102"/>
-      <c r="W3" s="102"/>
-      <c r="X3" s="102"/>
-      <c r="Y3" s="100"/>
-      <c r="Z3" s="100"/>
-      <c r="AA3" s="100"/>
-      <c r="AB3" s="100"/>
+      <c r="T3" s="99"/>
+      <c r="U3" s="99"/>
+      <c r="V3" s="99"/>
+      <c r="W3" s="99"/>
+      <c r="X3" s="99"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
@@ -2759,7 +2750,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="27">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="E13" s="65">
         <f>E9</f>
@@ -3154,7 +3145,7 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="58"/>
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="84" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="72" t="s">
@@ -3703,7 +3694,7 @@
         <v>45</v>
       </c>
       <c r="D25" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="67">
         <f>E9</f>
@@ -3784,7 +3775,7 @@
         <v>45</v>
       </c>
       <c r="D26" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="67">
         <f>F25</f>
@@ -4183,7 +4174,7 @@
         <v>44</v>
       </c>
       <c r="D31" s="37">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="E31" s="67">
         <f>E13</f>
@@ -4261,7 +4252,7 @@
         <v>45</v>
       </c>
       <c r="D32" s="37">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="E32" s="67">
         <f>F29</f>

</xml_diff>

<commit_message>
Forgetting to include some files
These files are not really necessary for the project, but I'll put 'em up anyeay,
</commit_message>
<xml_diff>
--- a/Week 7 Gantt Chart.xlsx
+++ b/Week 7 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{069BA28C-D5F5-4D3D-8FB0-4597D0772E53}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAE3F105-650E-459E-8332-411CC6D42045}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1619,8 +1619,8 @@
   <dimension ref="A1:BL42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding Warning to Exporting Files to the Front-End
Also added some comments to the Back-End
</commit_message>
<xml_diff>
--- a/Week 7 Gantt Chart.xlsx
+++ b/Week 7 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAE3F105-650E-459E-8332-411CC6D42045}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE03B79A-9138-4E40-BEAD-C8BE77F1FC76}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1619,8 +1619,8 @@
   <dimension ref="A1:BL42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2433,7 +2433,7 @@
         <v>45</v>
       </c>
       <c r="D9" s="22">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E9" s="64">
         <v>44980</v>
@@ -3937,7 +3937,7 @@
         <v>45</v>
       </c>
       <c r="D28" s="37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="67">
         <f>F26</f>
@@ -4252,7 +4252,7 @@
         <v>45</v>
       </c>
       <c r="D32" s="37">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="E32" s="67">
         <f>F29</f>
@@ -4486,7 +4486,7 @@
         <v>45</v>
       </c>
       <c r="D35" s="37">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E35" s="67">
         <f>E9</f>
@@ -4918,7 +4918,7 @@
     <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="I1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <printOptions horizontalCentered="1"/>
+  <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="95" fitToWidth="0" orientation="landscape" r:id="rId3"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">

</xml_diff>

<commit_message>
Updating Database to be more stable
So I found an issue in my database design that allowed for a few columns to be NULL when we always expect them to have a valid value. This lead to a few bad records sneaking into the database and causing problems. 

This commit is me deleting those records and remaking the BOOKS table to not allow NULLs in any of our columns except for Description and Genre.

Also updating the Gantt chart on my end to reflect the work that Mike did today.
</commit_message>
<xml_diff>
--- a/Week 7 Gantt Chart.xlsx
+++ b/Week 7 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="122" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE03B79A-9138-4E40-BEAD-C8BE77F1FC76}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7CA9CE2-6BA9-47CC-B3DB-ED44A421BA91}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1619,8 +1619,8 @@
   <dimension ref="A1:BL42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2831,7 +2831,7 @@
         <v>46</v>
       </c>
       <c r="D14" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="65">
         <f>E9+2</f>
@@ -2993,7 +2993,7 @@
         <v>46</v>
       </c>
       <c r="D16" s="27">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="E16" s="65">
         <f>F14</f>

</xml_diff>

<commit_message>
Cleaning up Code, Comments, and Unneeded Files for easier viewing
This is basically me getting rid of everything that we either don't need or we're not using or is not important.
</commit_message>
<xml_diff>
--- a/Week 7 Gantt Chart.xlsx
+++ b/Week 7 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="124" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7CA9CE2-6BA9-47CC-B3DB-ED44A421BA91}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10D16325-7680-4746-A8B2-8D4B5DA254D2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1619,8 +1619,8 @@
   <dimension ref="A1:BL42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4330,7 +4330,7 @@
         <v>45</v>
       </c>
       <c r="D33" s="37">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="E33" s="67">
         <f>F30</f>
@@ -4408,7 +4408,7 @@
         <v>45</v>
       </c>
       <c r="D34" s="37">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="E34" s="67">
         <f>F33</f>
@@ -4486,7 +4486,7 @@
         <v>45</v>
       </c>
       <c r="D35" s="37">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="E35" s="67">
         <f>E9</f>

</xml_diff>

<commit_message>
Updating the Documentation and Paperwork
</commit_message>
<xml_diff>
--- a/Week 7 Gantt Chart.xlsx
+++ b/Week 7 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="127" documentId="8_{91B8015C-2AD8-4214-8861-C67B5F7B4C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10D16325-7680-4746-A8B2-8D4B5DA254D2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED30DD8-F24A-4D46-BE0D-06E0CFAD93B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1348,10 +1348,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1619,8 +1615,8 @@
   <dimension ref="A1:BL42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3074,7 +3070,7 @@
         <v>46</v>
       </c>
       <c r="D17" s="27">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E17" s="65">
         <f>F16</f>
@@ -3308,7 +3304,7 @@
         <v>46</v>
       </c>
       <c r="D20" s="27">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E20" s="65">
         <f>F17</f>
@@ -3459,7 +3455,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="32">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E22" s="66">
         <f>F20+1</f>

</xml_diff>

<commit_message>
Bug fix to Back-End querying
</commit_message>
<xml_diff>
--- a/Week 7 Gantt Chart.xlsx
+++ b/Week 7 Gantt Chart.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED30DD8-F24A-4D46-BE0D-06E0CFAD93B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C3A690-DF64-4ED2-B685-D14260F70C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1615,8 +1615,8 @@
   <dimension ref="A1:BL42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2746,7 +2746,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="27">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E13" s="65">
         <f>E9</f>
@@ -2908,7 +2908,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="65">
         <f>F13</f>
@@ -3070,7 +3070,7 @@
         <v>46</v>
       </c>
       <c r="D17" s="27">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E17" s="65">
         <f>F16</f>
@@ -3148,7 +3148,7 @@
         <v>44</v>
       </c>
       <c r="D18" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="65">
         <f>F15</f>
@@ -3226,7 +3226,7 @@
         <v>44</v>
       </c>
       <c r="D19" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="65">
         <f>F18</f>
@@ -3304,7 +3304,7 @@
         <v>46</v>
       </c>
       <c r="D20" s="27">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E20" s="65">
         <f>F17</f>
@@ -3455,7 +3455,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="32">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="66">
         <f>F20+1</f>
@@ -3536,7 +3536,7 @@
         <v>44</v>
       </c>
       <c r="D23" s="32">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E23" s="66">
         <f>F19+1</f>
@@ -4170,7 +4170,7 @@
         <v>44</v>
       </c>
       <c r="D31" s="37">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E31" s="67">
         <f>E13</f>
@@ -4482,7 +4482,7 @@
         <v>45</v>
       </c>
       <c r="D35" s="37">
-        <v>0.6</v>
+        <v>0.35</v>
       </c>
       <c r="E35" s="67">
         <f>E9</f>

</xml_diff>

<commit_message>
Updating the Paperwork & Creating the Turn In File
</commit_message>
<xml_diff>
--- a/Week 7 Gantt Chart.xlsx
+++ b/Week 7 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C3A690-DF64-4ED2-B685-D14260F70C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673193FA-A06E-412B-A97D-7DDF0CB4B236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1615,8 +1615,8 @@
   <dimension ref="A1:BL42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL3" sqref="AL3"/>
+      <pane ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3455,7 +3455,7 @@
         <v>46</v>
       </c>
       <c r="D22" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E22" s="66">
         <f>F20+1</f>
@@ -3536,7 +3536,7 @@
         <v>44</v>
       </c>
       <c r="D23" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E23" s="66">
         <f>F19+1</f>
@@ -4916,7 +4916,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="95" fitToWidth="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="70" fitToWidth="0" orientation="portrait" r:id="rId3"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>